<commit_message>
manage demultiplexed reads. Look for existing R1,R2,I1,I2 files in path defined in the sample datasheet for each sample. A symlink is generated from path to 00-demultiplexing/ folder
</commit_message>
<xml_diff>
--- a/test_dataset/test_datasheet.xlsx
+++ b/test_dataset/test_datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://institut-my.sharepoint.com/personal/gcorre_genethon_fr/Documents/Bureau/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Eq_UDG\bioinformatique\01-pipelines\omics\ShortReadSequencing\GuideSeq\GUIDE-Seq_genethon\test_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D95F6B52-BF95-46B8-AF06-91382A5C5CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D52D52-9CEA-4D11-AFEF-A5F0CA9F4F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A849A2B9-5AEE-407F-80B9-CAB473E64C7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A849A2B9-5AEE-407F-80B9-CAB473E64C7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>sampleName</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>CTAAGC</t>
+  </si>
+  <si>
+    <t>/media/Data/common/guideseq_gnt_dev/test_dataset/</t>
+  </si>
+  <si>
+    <t>path_to_files</t>
   </si>
 </sst>
 </file>
@@ -494,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4ACCEC-A3C9-495B-9DB4-02B207EEC8AA}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,8 +551,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -586,8 +595,11 @@
       <c r="N2" t="s">
         <v>23</v>
       </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -626,6 +638,9 @@
       </c>
       <c r="N3" t="s">
         <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>